<commit_message>
revisão entrega trabalho final
</commit_message>
<xml_diff>
--- a/dados/covid_19_bauru_casos_geral.xlsx
+++ b/dados/covid_19_bauru_casos_geral.xlsx
@@ -8,14 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpalbino/Library/Mobile Documents/com~apple~CloudDocs/GitHub/covid19-bauru/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBFB098-BB76-AA4D-B9C7-DAC19DA4CB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5FE606-9502-A04A-A012-EDDB3BA0C990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12280" yWindow="500" windowWidth="16280" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="covid_19_bauru_casos_geral" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -926,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N478"/>
+  <dimension ref="A1:N482"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
-      <selection activeCell="K481" sqref="K481"/>
+      <selection activeCell="E484" sqref="E484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16552,6 +16564,167 @@
         <v>75</v>
       </c>
     </row>
+    <row r="479" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A479" s="3">
+        <v>44628</v>
+      </c>
+      <c r="B479" s="2">
+        <v>12</v>
+      </c>
+      <c r="C479" s="2">
+        <v>81433</v>
+      </c>
+      <c r="D479" s="2">
+        <v>1376</v>
+      </c>
+      <c r="E479" s="2">
+        <v>3</v>
+      </c>
+      <c r="F479" s="2">
+        <v>3</v>
+      </c>
+      <c r="G479" s="2">
+        <v>75815</v>
+      </c>
+      <c r="H479" s="2">
+        <v>134071</v>
+      </c>
+      <c r="I479" s="2">
+        <v>215507</v>
+      </c>
+      <c r="J479" s="2">
+        <v>10</v>
+      </c>
+      <c r="K479" s="2">
+        <v>8</v>
+      </c>
+      <c r="L479" s="2">
+        <v>75</v>
+      </c>
+      <c r="M479" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="480" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A480" s="3">
+        <v>44629</v>
+      </c>
+      <c r="B480" s="2">
+        <v>10</v>
+      </c>
+      <c r="C480" s="2">
+        <v>81443</v>
+      </c>
+      <c r="D480" s="2">
+        <v>1378</v>
+      </c>
+      <c r="E480" s="2">
+        <v>2</v>
+      </c>
+      <c r="F480" s="2">
+        <v>18</v>
+      </c>
+      <c r="G480" s="2">
+        <v>76210</v>
+      </c>
+      <c r="H480" s="2">
+        <v>134195</v>
+      </c>
+      <c r="I480" s="2">
+        <v>215656</v>
+      </c>
+      <c r="J480" s="2">
+        <v>10</v>
+      </c>
+      <c r="K480" s="2">
+        <v>7</v>
+      </c>
+      <c r="L480" s="2">
+        <v>75</v>
+      </c>
+      <c r="M480" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="481" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A481" s="3">
+        <v>44630</v>
+      </c>
+      <c r="B481" s="2">
+        <v>7</v>
+      </c>
+      <c r="C481" s="2">
+        <v>81450</v>
+      </c>
+      <c r="D481" s="2">
+        <v>1379</v>
+      </c>
+      <c r="E481" s="2">
+        <v>1</v>
+      </c>
+      <c r="F481" s="2">
+        <v>3</v>
+      </c>
+      <c r="G481" s="2">
+        <v>76475</v>
+      </c>
+      <c r="H481" s="2">
+        <v>134286</v>
+      </c>
+      <c r="J481" s="2">
+        <v>10</v>
+      </c>
+      <c r="K481" s="2">
+        <v>7</v>
+      </c>
+      <c r="L481" s="2">
+        <v>75</v>
+      </c>
+      <c r="M481" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="482" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A482" s="3">
+        <v>44631</v>
+      </c>
+      <c r="B482" s="2">
+        <v>3</v>
+      </c>
+      <c r="C482" s="2">
+        <v>81453</v>
+      </c>
+      <c r="D482" s="2">
+        <v>1381</v>
+      </c>
+      <c r="E482" s="2">
+        <v>1</v>
+      </c>
+      <c r="F482" s="2">
+        <v>5</v>
+      </c>
+      <c r="G482" s="2">
+        <v>76715</v>
+      </c>
+      <c r="H482" s="2">
+        <v>134718</v>
+      </c>
+      <c r="I482" s="2">
+        <v>216176</v>
+      </c>
+      <c r="J482" s="2">
+        <v>10</v>
+      </c>
+      <c r="K482" s="2">
+        <v>3</v>
+      </c>
+      <c r="L482" s="2">
+        <v>75</v>
+      </c>
+      <c r="M482" s="2">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>